<commit_message>
#327 Ajout des profils d'acces a58d18c1e8091c98efec92c8c093b361a253eee5
</commit_message>
<xml_diff>
--- a/327-automatisation-mapping/ig/StructureDefinition-RORPractitionerRoleName.xlsx
+++ b/327-automatisation-mapping/ig/StructureDefinition-RORPractitionerRoleName.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-14T13:39:21+00:00</t>
+    <t>2024-03-19T13:17:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -237,10 +237,10 @@
     <t>Constraint(s)</t>
   </si>
   <si>
+    <t>Mapping: Spécification métier vers l'extension ROR RORPractitionerRoleName</t>
+  </si>
+  <si>
     <t>Mapping: RIM Mapping</t>
-  </si>
-  <si>
-    <t>Mapping: Spécification métier vers l'extension ROR RORPractitionerRoleName</t>
   </si>
   <si>
     <t/>
@@ -795,8 +795,8 @@
     <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="24.98046875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="82.18359375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="82.18359375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="24.98046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1121,10 +1121,10 @@
         <v>76</v>
       </c>
       <c r="AK3" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL3" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AL3" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="4">
@@ -1441,10 +1441,10 @@
         <v>76</v>
       </c>
       <c r="AK6" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL6" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AL6" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="7">
@@ -1655,10 +1655,10 @@
         <v>76</v>
       </c>
       <c r="AK8" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL8" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL8" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="9">
@@ -1759,10 +1759,10 @@
         <v>118</v>
       </c>
       <c r="AK9" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL9" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL9" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="10">
@@ -1865,10 +1865,10 @@
         <v>118</v>
       </c>
       <c r="AK10" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="AL10" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL10" t="s" s="2">
-        <v>123</v>
       </c>
     </row>
     <row r="11">
@@ -2079,10 +2079,10 @@
         <v>76</v>
       </c>
       <c r="AK12" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL12" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AL12" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -2293,10 +2293,10 @@
         <v>76</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL14" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -2399,10 +2399,10 @@
         <v>118</v>
       </c>
       <c r="AK15" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AL15" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL15" t="s" s="2">
-        <v>130</v>
       </c>
     </row>
     <row r="16">
@@ -2613,10 +2613,10 @@
         <v>76</v>
       </c>
       <c r="AK17" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>88</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -2827,10 +2827,10 @@
         <v>76</v>
       </c>
       <c r="AK19" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL19" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL19" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -2933,10 +2933,10 @@
         <v>118</v>
       </c>
       <c r="AK20" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>137</v>
       </c>
     </row>
     <row r="21">
@@ -3041,10 +3041,10 @@
         <v>76</v>
       </c>
       <c r="AK21" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
     <row r="22">
@@ -3147,10 +3147,10 @@
         <v>118</v>
       </c>
       <c r="AK22" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL22" t="s" s="2">
         <v>109</v>
-      </c>
-      <c r="AL22" t="s" s="2">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>